<commit_message>
Sprint reflectie toegevoegd aan sprintplan
</commit_message>
<xml_diff>
--- a/SE Deliverables/Week 1/Sprint_1_24.4.2015/Sprintplan 1.xlsx
+++ b/SE Deliverables/Week 1/Sprint_1_24.4.2015/Sprintplan 1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Werkblad 1 - Sprint Plan #1_x0009_Gam" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>User Story</t>
   </si>
@@ -102,9 +102,6 @@
     <t>finding out how GAM works (checking code + documentation) and summarize</t>
   </si>
   <si>
-    <t>NOTE: This week we will probably all work out how these software implementations work so we weren't able to decice very specifically what we will do.</t>
-  </si>
-  <si>
     <t>Bernd (working with Rolf)</t>
   </si>
   <si>
@@ -118,6 +115,37 @@
   </si>
   <si>
     <t>priority (1&gt;2&gt;3)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>We did this by implementing a first and second game</t>
+  </si>
+  <si>
+    <t>Product vision document</t>
+  </si>
+  <si>
+    <t>Client meeting</t>
+  </si>
+  <si>
+    <t>NOTE: This week we will probably all work out how these software implementations work so we weren't able to decice very specifically what we will do.
+This week we only had 2,5 project blocks where we could actually work on the project, the other blocks were occupied with a free day or classes.</t>
+  </si>
+  <si>
+    <t>Task completed by</t>
+  </si>
+  <si>
+    <t>Everybody</t>
+  </si>
+  <si>
+    <t>Max and Bernd</t>
+  </si>
+  <si>
+    <t>Joost and Yannick</t>
+  </si>
+  <si>
+    <t>Noone</t>
   </si>
 </sst>
 </file>
@@ -183,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -227,17 +255,34 @@
         <color indexed="8"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
@@ -261,7 +306,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -283,16 +328,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -376,6 +424,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1624,35 +1677,39 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW21"/>
+  <dimension ref="A1:IX21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.25" style="1" customWidth="1"/>
-    <col min="9" max="257" width="9" style="1" customWidth="1"/>
+    <col min="1" max="2" width="22" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="258" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="36">
+    <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1663,22 +1720,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24">
+    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -1688,19 +1748,26 @@
       <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>5</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4">
+        <v>4</v>
+      </c>
       <c r="H3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16">
+    <row r="4" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1708,75 +1775,103 @@
       <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
       <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1">
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="4">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>20</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4">
+        <v>20</v>
+      </c>
       <c r="H6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="4">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>15</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="4">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1">
+    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1785,8 +1880,9 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="36">
+    <row r="9" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1796,17 +1892,24 @@
       <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>4</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1">
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
@@ -1814,46 +1917,65 @@
       <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>15</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A11" s="9"/>
+    <row r="11" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="4">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>5</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="4"/>
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="44.25" customHeight="1">
-      <c r="A13" s="11"/>
+    <row r="13" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1861,28 +1983,55 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1">
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1">
+    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1">
+    <row r="16" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1891,8 +2040,9 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1">
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1901,8 +2051,9 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1">
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1911,8 +2062,9 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="16">
+    <row r="19" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1921,34 +2073,38 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="36">
+    <row r="20" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4">
-        <f>SUM(E3:E11)</f>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4">
+        <f>SUM(F3:F11)</f>
         <v>72</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4" t="s">
-        <v>27</v>
+      <c r="G20" s="4">
+        <f>SUM(G3:G19)</f>
+        <v>57.5</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="77" customHeight="1">
+    <row r="21" spans="1:9" ht="76.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A11:A13"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>